<commit_message>
Updated TIming and Dosage
</commit_message>
<xml_diff>
--- a/Mappings/Medicatie9.xlsx
+++ b/Mappings/Medicatie9.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\MedMij-STU3\Mappings\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\Nictiz-STU3\Mappings\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7800" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7800"/>
   </bookViews>
   <sheets>
     <sheet name="MedicatieAfspraak" sheetId="2" r:id="rId1"/>
@@ -817,15 +817,6 @@
     <t>MedicationRequest.dosageInstructions.additionalInstructions</t>
   </si>
   <si>
-    <t>MedicationRequest.dosageInstructions.quantityRange.low</t>
-  </si>
-  <si>
-    <t>MedicationRequest.dosageInstructions.quantityQuantity</t>
-  </si>
-  <si>
-    <t>MedicationRequest.dosageInstructions.quantityRange.high</t>
-  </si>
-  <si>
     <t>MedicationRequest.authoredOn</t>
   </si>
   <si>
@@ -1097,6 +1088,15 @@
   </si>
   <si>
     <t>MedicationRequest.extension (string)</t>
+  </si>
+  <si>
+    <t>MedicationRequest.dosageInstructions.doseRange.low</t>
+  </si>
+  <si>
+    <t>MedicationRequest.dosageInstructions.doseQuantity</t>
+  </si>
+  <si>
+    <t>MedicationRequest.dosageInstructions.doseRange.high</t>
   </si>
 </sst>
 </file>
@@ -1400,9 +1400,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
@@ -1445,6 +1442,9 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1786,8 +1786,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L88"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40:G40"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G62" sqref="G62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1"/>
@@ -1804,16 +1804,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="52" t="s">
         <v>152</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
       <c r="I1" s="1" t="s">
         <v>132</v>
       </c>
@@ -1861,7 +1861,7 @@
         <v>19</v>
       </c>
       <c r="K4" s="32" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -1917,7 +1917,7 @@
         <v>21</v>
       </c>
       <c r="K8" s="25" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -1943,7 +1943,7 @@
       </c>
       <c r="J10" s="2"/>
       <c r="K10" s="26" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="11" spans="1:12" hidden="1" outlineLevel="1">
@@ -2113,7 +2113,7 @@
         <v>8</v>
       </c>
       <c r="K25" s="25" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="26" spans="2:11">
@@ -2196,7 +2196,7 @@
         <v>8</v>
       </c>
       <c r="K31" s="18" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="32" spans="2:11">
@@ -2209,7 +2209,7 @@
       </c>
       <c r="J32" s="2"/>
       <c r="K32" s="18" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="33" spans="1:12">
@@ -2233,7 +2233,7 @@
       </c>
       <c r="J34" s="2"/>
       <c r="K34" s="18" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="35" spans="1:12">
@@ -2313,7 +2313,7 @@
         <v>8</v>
       </c>
       <c r="K40" s="18" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="41" spans="1:12">
@@ -2326,7 +2326,7 @@
       </c>
       <c r="J41" s="2"/>
       <c r="K41" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="42" spans="1:12">
@@ -2411,8 +2411,8 @@
       <c r="J47" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="K47" s="36" t="s">
-        <v>273</v>
+      <c r="K47" s="35" t="s">
+        <v>270</v>
       </c>
       <c r="L47" t="s">
         <v>219</v>
@@ -2478,7 +2478,7 @@
         <v>52</v>
       </c>
       <c r="K52" s="21" t="s">
-        <v>262</v>
+        <v>353</v>
       </c>
     </row>
     <row r="53" spans="1:11">
@@ -2493,7 +2493,7 @@
         <v>52</v>
       </c>
       <c r="K53" s="21" t="s">
-        <v>263</v>
+        <v>354</v>
       </c>
     </row>
     <row r="54" spans="1:11">
@@ -2508,7 +2508,7 @@
         <v>52</v>
       </c>
       <c r="K54" s="21" t="s">
-        <v>264</v>
+        <v>355</v>
       </c>
     </row>
     <row r="55" spans="1:11">
@@ -2661,7 +2661,7 @@
         <v>8</v>
       </c>
       <c r="K65" s="10" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="66" spans="1:11">
@@ -2675,7 +2675,7 @@
       <c r="J66" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="K66" s="36" t="s">
+      <c r="K66" s="35" t="s">
         <v>247</v>
       </c>
     </row>
@@ -2742,8 +2742,8 @@
         <v>3</v>
       </c>
       <c r="J71" s="2"/>
-      <c r="K71" s="37" t="s">
-        <v>275</v>
+      <c r="K71" s="36" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="72" spans="1:11">
@@ -2758,7 +2758,7 @@
         <v>31</v>
       </c>
       <c r="K72" s="10" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="73" spans="1:11">
@@ -2773,7 +2773,7 @@
         <v>8</v>
       </c>
       <c r="K73" s="10" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="74" spans="1:11">
@@ -2788,7 +2788,7 @@
         <v>8</v>
       </c>
       <c r="K74" s="10" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="75" spans="1:11">
@@ -2897,8 +2897,8 @@
         <v>3</v>
       </c>
       <c r="J82" s="2"/>
-      <c r="K82" s="38" t="s">
-        <v>279</v>
+      <c r="K82" s="37" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="83" spans="2:11">
@@ -2933,8 +2933,8 @@
         <v>3</v>
       </c>
       <c r="J85" s="2"/>
-      <c r="K85" s="38" t="s">
-        <v>279</v>
+      <c r="K85" s="37" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="86" spans="2:11">
@@ -3007,16 +3007,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="52" t="s">
         <v>152</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
       <c r="I1" s="1" t="s">
         <v>132</v>
       </c>
@@ -3080,11 +3080,11 @@
       <c r="J5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="K5" s="40" t="s">
-        <v>280</v>
+      <c r="K5" s="39" t="s">
+        <v>277</v>
       </c>
       <c r="L5" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -3152,7 +3152,7 @@
       </c>
       <c r="J10" s="2"/>
       <c r="K10" s="26" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -3218,7 +3218,7 @@
         <v>8</v>
       </c>
       <c r="K15" s="18" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -3230,7 +3230,7 @@
       </c>
       <c r="J16" s="2"/>
       <c r="K16" s="18" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -3252,7 +3252,7 @@
       </c>
       <c r="J18" s="2"/>
       <c r="K18" s="18" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -3327,7 +3327,7 @@
         <v>8</v>
       </c>
       <c r="K24" s="18" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="25" spans="1:11">
@@ -3339,7 +3339,7 @@
       </c>
       <c r="J25" s="2"/>
       <c r="K25" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="26" spans="1:11">
@@ -3353,7 +3353,7 @@
         <v>4</v>
       </c>
       <c r="K26" s="18" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="27" spans="1:11">
@@ -3367,7 +3367,7 @@
         <v>8</v>
       </c>
       <c r="K27" s="18" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="28" spans="1:11">
@@ -3381,7 +3381,7 @@
         <v>4</v>
       </c>
       <c r="K28" s="18" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
     <row r="29" spans="1:11">
@@ -3395,7 +3395,7 @@
         <v>31</v>
       </c>
       <c r="K29" s="10" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
     </row>
     <row r="30" spans="1:11">
@@ -3418,8 +3418,8 @@
       <c r="J31" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="K31" s="36" t="s">
-        <v>295</v>
+      <c r="K31" s="35" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="32" spans="1:11">
@@ -3433,7 +3433,7 @@
         <v>31</v>
       </c>
       <c r="K32" s="10" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
     </row>
     <row r="33" spans="3:11">
@@ -3477,7 +3477,7 @@
         <v>52</v>
       </c>
       <c r="K36" s="21" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="37" spans="3:11">
@@ -3491,7 +3491,7 @@
         <v>52</v>
       </c>
       <c r="K37" s="21" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="38" spans="3:11">
@@ -3505,7 +3505,7 @@
         <v>52</v>
       </c>
       <c r="K38" s="21" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
     </row>
     <row r="39" spans="3:11">
@@ -3519,7 +3519,7 @@
         <v>8</v>
       </c>
       <c r="K39" s="11" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="40" spans="3:11">
@@ -3577,7 +3577,7 @@
         <v>52</v>
       </c>
       <c r="K44" s="10" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="45" spans="3:11">
@@ -3591,7 +3591,7 @@
         <v>52</v>
       </c>
       <c r="K45" s="10" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="46" spans="3:11">
@@ -3605,7 +3605,7 @@
         <v>52</v>
       </c>
       <c r="K46" s="10" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
     </row>
     <row r="47" spans="3:11">
@@ -3619,7 +3619,7 @@
         <v>8</v>
       </c>
       <c r="K47" s="10" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="48" spans="3:11">
@@ -3633,7 +3633,7 @@
         <v>31</v>
       </c>
       <c r="K48" s="10" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
     </row>
     <row r="49" spans="5:11">
@@ -3647,7 +3647,7 @@
         <v>19</v>
       </c>
       <c r="K49" s="10" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="50" spans="5:11">
@@ -3661,7 +3661,7 @@
         <v>8</v>
       </c>
       <c r="K50" s="10" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
     </row>
     <row r="51" spans="5:11">
@@ -3674,8 +3674,8 @@
       <c r="J51" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="K51" s="36" t="s">
-        <v>305</v>
+      <c r="K51" s="35" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="52" spans="5:11">
@@ -3687,7 +3687,7 @@
       </c>
       <c r="J52" s="2"/>
       <c r="K52" s="18" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
     </row>
     <row r="53" spans="5:11">
@@ -3711,7 +3711,7 @@
         <v>8</v>
       </c>
       <c r="K54" s="18" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
     </row>
     <row r="55" spans="5:11">
@@ -3725,7 +3725,7 @@
         <v>4</v>
       </c>
       <c r="K55" s="18" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="56" spans="5:11">
@@ -3736,8 +3736,8 @@
         <v>3</v>
       </c>
       <c r="J56" s="2"/>
-      <c r="K56" s="37" t="s">
-        <v>309</v>
+      <c r="K56" s="36" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="57" spans="5:11">
@@ -3751,7 +3751,7 @@
         <v>31</v>
       </c>
       <c r="K57" s="10" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="58" spans="5:11">
@@ -3765,7 +3765,7 @@
         <v>8</v>
       </c>
       <c r="K58" s="10" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="59" spans="5:11">
@@ -3779,7 +3779,7 @@
         <v>8</v>
       </c>
       <c r="K59" s="10" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="60" spans="5:11">
@@ -3791,7 +3791,7 @@
       </c>
       <c r="J60" s="2"/>
       <c r="K60" s="10" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
     </row>
     <row r="61" spans="5:11">
@@ -3815,7 +3815,7 @@
         <v>52</v>
       </c>
       <c r="K62" s="10" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
     </row>
     <row r="63" spans="5:11">
@@ -3829,7 +3829,7 @@
         <v>52</v>
       </c>
       <c r="K63" s="10" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
     </row>
     <row r="64" spans="5:11">
@@ -3843,7 +3843,7 @@
         <v>52</v>
       </c>
       <c r="K64" s="10" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
     </row>
     <row r="65" spans="2:11">
@@ -3883,22 +3883,22 @@
       </c>
       <c r="J67" s="2"/>
       <c r="K67" s="23" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="68" spans="2:11" s="39" customFormat="1">
-      <c r="B68" s="42"/>
-      <c r="C68" s="42" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="68" spans="2:11" s="38" customFormat="1">
+      <c r="B68" s="41"/>
+      <c r="C68" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="I68" s="43" t="s">
-        <v>3</v>
-      </c>
-      <c r="J68" s="43" t="s">
+      <c r="I68" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="J68" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="K68" s="44" t="s">
-        <v>286</v>
+      <c r="K68" s="43" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="69" spans="2:11">
@@ -3910,34 +3910,34 @@
       </c>
       <c r="J69" s="2"/>
       <c r="K69" s="23" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="70" spans="2:11" s="39" customFormat="1">
-      <c r="B70" s="42"/>
-      <c r="C70" s="42" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="70" spans="2:11" s="38" customFormat="1">
+      <c r="B70" s="41"/>
+      <c r="C70" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="I70" s="43" t="s">
-        <v>3</v>
-      </c>
-      <c r="J70" s="43" t="s">
+      <c r="I70" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="J70" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="K70" s="44" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="71" spans="2:11" s="39" customFormat="1">
-      <c r="B71" s="39" t="s">
+      <c r="K70" s="43" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="71" spans="2:11" s="38" customFormat="1">
+      <c r="B71" s="38" t="s">
         <v>73</v>
       </c>
-      <c r="I71" s="43" t="s">
-        <v>3</v>
-      </c>
-      <c r="J71" s="43"/>
-      <c r="K71" s="44" t="s">
-        <v>283</v>
+      <c r="I71" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="J71" s="42"/>
+      <c r="K71" s="43" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="72" spans="2:11" hidden="1" outlineLevel="2">
@@ -4427,9 +4427,9 @@
         <v>4</v>
       </c>
       <c r="K113" s="10" t="s">
-        <v>284</v>
-      </c>
-      <c r="L113" s="41"/>
+        <v>281</v>
+      </c>
+      <c r="L113" s="40"/>
     </row>
     <row r="114" spans="2:12">
       <c r="B114" s="3" t="s">
@@ -4500,16 +4500,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="18" customHeight="1">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="52" t="s">
         <v>152</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
       <c r="I1" s="1" t="s">
         <v>132</v>
       </c>
@@ -4554,7 +4554,7 @@
       </c>
       <c r="J4" s="2"/>
       <c r="K4" s="10" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="13.9" customHeight="1">
@@ -4608,7 +4608,7 @@
       <c r="K8" s="22" t="s">
         <v>160</v>
       </c>
-      <c r="L8" s="45"/>
+      <c r="L8" s="44"/>
     </row>
     <row r="9" spans="1:14" ht="13.15" customHeight="1">
       <c r="E9" s="3" t="s">
@@ -4621,7 +4621,7 @@
         <v>8</v>
       </c>
       <c r="K9" s="18" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="10" spans="1:14">
@@ -4633,7 +4633,7 @@
       </c>
       <c r="J10" s="2"/>
       <c r="K10" s="18" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="11" spans="1:14">
@@ -4645,7 +4645,7 @@
       </c>
       <c r="J11" s="2"/>
       <c r="K11" s="18" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="16.149999999999999" customHeight="1">
@@ -4678,7 +4678,7 @@
         <v>8</v>
       </c>
       <c r="K14" s="18" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="15" spans="1:14">
@@ -4703,16 +4703,16 @@
     </row>
     <row r="16" spans="1:14">
       <c r="B16" s="3" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="J16" s="4" t="s">
         <v>21</v>
       </c>
       <c r="K16" s="19" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
     </row>
     <row r="17" spans="2:14">
@@ -4765,7 +4765,7 @@
       <c r="J19" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="K19" s="46" t="s">
+      <c r="K19" s="45" t="s">
         <v>181</v>
       </c>
       <c r="M19" s="27" t="s">
@@ -4777,16 +4777,16 @@
     </row>
     <row r="20" spans="2:14">
       <c r="B20" s="3" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="J20" s="4" t="s">
         <v>21</v>
       </c>
       <c r="K20" s="34" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="M20" s="27"/>
       <c r="N20" s="27"/>
@@ -4820,22 +4820,22 @@
       </c>
       <c r="J22" s="2"/>
       <c r="K22" s="23" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="23" spans="2:14" s="39" customFormat="1">
-      <c r="B23" s="42"/>
-      <c r="C23" s="42" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="23" spans="2:14" s="38" customFormat="1">
+      <c r="B23" s="41"/>
+      <c r="C23" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="I23" s="43" t="s">
-        <v>3</v>
-      </c>
-      <c r="J23" s="43" t="s">
+      <c r="I23" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="J23" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="K23" s="44" t="s">
-        <v>286</v>
+      <c r="K23" s="43" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="24" spans="2:14">
@@ -4863,7 +4863,7 @@
       </c>
       <c r="J25" s="2"/>
       <c r="K25" s="25" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
     </row>
     <row r="26" spans="2:14" hidden="1" outlineLevel="1">
@@ -5074,7 +5074,7 @@
       </c>
       <c r="J43" s="2"/>
       <c r="K43" s="25" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
     <row r="44" spans="3:11" hidden="1" outlineLevel="2">
@@ -5509,16 +5509,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="52" t="s">
         <v>152</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
       <c r="I1" s="1" t="s">
         <v>132</v>
       </c>
@@ -5554,8 +5554,8 @@
       <c r="J3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="K3" s="47" t="s">
-        <v>330</v>
+      <c r="K3" s="46" t="s">
+        <v>327</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -5616,7 +5616,7 @@
     </row>
     <row r="8" spans="1:12">
       <c r="B8" s="3" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="I8" s="4" t="s">
         <v>3</v>
@@ -5624,8 +5624,8 @@
       <c r="J8" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="K8" s="47" t="s">
-        <v>343</v>
+      <c r="K8" s="46" t="s">
+        <v>340</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -5638,8 +5638,8 @@
       <c r="J9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="K9" s="47" t="s">
-        <v>344</v>
+      <c r="K9" s="46" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -5650,8 +5650,8 @@
         <v>0</v>
       </c>
       <c r="J10" s="2"/>
-      <c r="K10" s="47" t="s">
-        <v>331</v>
+      <c r="K10" s="46" t="s">
+        <v>328</v>
       </c>
       <c r="L10" t="s">
         <v>207</v>
@@ -5665,8 +5665,8 @@
         <v>3</v>
       </c>
       <c r="J11" s="2"/>
-      <c r="K11" s="47" t="s">
-        <v>332</v>
+      <c r="K11" s="46" t="s">
+        <v>329</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -5726,7 +5726,7 @@
       </c>
       <c r="J16" s="2"/>
       <c r="K16" s="26" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -5802,7 +5802,7 @@
         <v>8</v>
       </c>
       <c r="K22" s="18" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="23" spans="1:11">
@@ -5814,7 +5814,7 @@
       </c>
       <c r="J23" s="2"/>
       <c r="K23" s="18" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="24" spans="1:11">
@@ -5836,7 +5836,7 @@
       </c>
       <c r="J25" s="2"/>
       <c r="K25" s="18" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="26" spans="1:11">
@@ -5910,7 +5910,7 @@
         <v>8</v>
       </c>
       <c r="K31" s="18" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="32" spans="1:11">
@@ -5923,7 +5923,7 @@
       </c>
       <c r="J32" s="2"/>
       <c r="K32" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="33" spans="1:11">
@@ -5968,7 +5968,7 @@
         <v>4</v>
       </c>
       <c r="K35" s="18" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="36" spans="1:11">
@@ -6008,8 +6008,8 @@
       <c r="J38" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="K38" s="36" t="s">
-        <v>339</v>
+      <c r="K38" s="35" t="s">
+        <v>336</v>
       </c>
     </row>
     <row r="39" spans="1:11">
@@ -6072,7 +6072,7 @@
         <v>52</v>
       </c>
       <c r="K43" s="21" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
     </row>
     <row r="44" spans="1:11">
@@ -6087,7 +6087,7 @@
         <v>52</v>
       </c>
       <c r="K44" s="21" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
     </row>
     <row r="45" spans="1:11">
@@ -6102,7 +6102,7 @@
         <v>52</v>
       </c>
       <c r="K45" s="21" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
     </row>
     <row r="46" spans="1:11">
@@ -6117,7 +6117,7 @@
         <v>8</v>
       </c>
       <c r="K46" s="11" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="47" spans="1:11">
@@ -6273,7 +6273,7 @@
         <v>8</v>
       </c>
       <c r="K57" s="10" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="58" spans="1:12">
@@ -6287,7 +6287,7 @@
       <c r="J58" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="K58" s="36" t="s">
+      <c r="K58" s="35" t="s">
         <v>228</v>
       </c>
     </row>
@@ -6354,8 +6354,8 @@
         <v>3</v>
       </c>
       <c r="J63" s="2"/>
-      <c r="K63" s="37" t="s">
-        <v>335</v>
+      <c r="K63" s="36" t="s">
+        <v>332</v>
       </c>
     </row>
     <row r="64" spans="1:12">
@@ -6370,7 +6370,7 @@
         <v>31</v>
       </c>
       <c r="K64" s="10" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="65" spans="1:12">
@@ -6385,7 +6385,7 @@
         <v>8</v>
       </c>
       <c r="K65" s="10" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="66" spans="1:12">
@@ -6400,7 +6400,7 @@
         <v>8</v>
       </c>
       <c r="K66" s="10" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="67" spans="1:12">
@@ -6504,12 +6504,12 @@
     </row>
     <row r="74" spans="1:12">
       <c r="A74" s="3"/>
-      <c r="B74" s="47" t="s">
-        <v>325</v>
-      </c>
-      <c r="C74" s="47"/>
-      <c r="D74" s="47"/>
-      <c r="E74" s="47"/>
+      <c r="B74" s="46" t="s">
+        <v>322</v>
+      </c>
+      <c r="C74" s="46"/>
+      <c r="D74" s="46"/>
+      <c r="E74" s="46"/>
       <c r="G74" s="3"/>
       <c r="I74" s="4" t="s">
         <v>3</v>
@@ -6554,7 +6554,7 @@
         <v>17</v>
       </c>
       <c r="K77" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="L77" t="s">
         <v>212</v>
@@ -6593,16 +6593,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="14.45" customHeight="1">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="52" t="s">
         <v>152</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
       <c r="I1" s="1" t="s">
         <v>132</v>
       </c>
@@ -6983,7 +6983,7 @@
       <c r="K29" s="29" t="s">
         <v>200</v>
       </c>
-      <c r="L29" s="39"/>
+      <c r="L29" s="38"/>
     </row>
     <row r="30" spans="2:12">
       <c r="B30" s="3" t="s">
@@ -7018,10 +7018,10 @@
     </row>
     <row r="32" spans="2:12">
       <c r="B32" s="3" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="J32" s="4" t="s">
         <v>4</v>
@@ -7029,7 +7029,7 @@
       <c r="K32" s="25" t="s">
         <v>201</v>
       </c>
-      <c r="L32" s="48"/>
+      <c r="L32" s="47"/>
     </row>
     <row r="33" spans="2:11">
       <c r="B33" s="3" t="s">
@@ -7084,7 +7084,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="K50" sqref="K50"/>
     </sheetView>
   </sheetViews>
@@ -7101,16 +7101,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="52" t="s">
         <v>152</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
       <c r="I1" s="1" t="s">
         <v>132</v>
       </c>
@@ -7173,7 +7173,7 @@
       </c>
       <c r="J5" s="2"/>
       <c r="K5" s="25" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
     </row>
     <row r="6" spans="1:12" hidden="1" outlineLevel="1">
@@ -7297,7 +7297,7 @@
       </c>
       <c r="J16" s="2"/>
       <c r="K16" s="25" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
     </row>
     <row r="17" spans="2:11">
@@ -7311,7 +7311,7 @@
         <v>31</v>
       </c>
       <c r="K17" s="25" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
     </row>
     <row r="18" spans="2:11">
@@ -7325,7 +7325,7 @@
         <v>8</v>
       </c>
       <c r="K18" s="25" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
     </row>
     <row r="19" spans="2:11">
@@ -7339,7 +7339,7 @@
         <v>52</v>
       </c>
       <c r="K19" s="25" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="20" spans="2:11">
@@ -7351,7 +7351,7 @@
       </c>
       <c r="J20" s="2"/>
       <c r="K20" s="26" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
     </row>
     <row r="21" spans="2:11">
@@ -7427,7 +7427,7 @@
         <v>8</v>
       </c>
       <c r="K26" s="18" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="27" spans="2:11">
@@ -7439,7 +7439,7 @@
       </c>
       <c r="J27" s="2"/>
       <c r="K27" s="18" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="28" spans="2:11">
@@ -7461,7 +7461,7 @@
       </c>
       <c r="J29" s="2"/>
       <c r="K29" s="18" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="30" spans="2:11">
@@ -7535,7 +7535,7 @@
         <v>8</v>
       </c>
       <c r="K35" s="18" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="36" spans="2:11">
@@ -7559,7 +7559,7 @@
         <v>19</v>
       </c>
       <c r="K37" s="25" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
     </row>
     <row r="38" spans="2:11">
@@ -7573,7 +7573,7 @@
         <v>149</v>
       </c>
       <c r="K38" s="25" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
     </row>
     <row r="39" spans="2:11">
@@ -7587,7 +7587,7 @@
         <v>19</v>
       </c>
       <c r="K39" s="25" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
     </row>
     <row r="40" spans="2:11">
@@ -7598,8 +7598,8 @@
         <v>3</v>
       </c>
       <c r="J40" s="2"/>
-      <c r="K40" s="52" t="s">
-        <v>354</v>
+      <c r="K40" s="51" t="s">
+        <v>351</v>
       </c>
     </row>
     <row r="41" spans="2:11">
@@ -7610,7 +7610,7 @@
         <v>0</v>
       </c>
       <c r="J41" s="2"/>
-      <c r="K41" s="49"/>
+      <c r="K41" s="48"/>
     </row>
     <row r="42" spans="2:11">
       <c r="D42" s="3" t="s">
@@ -7622,7 +7622,7 @@
       <c r="J42" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="K42" s="50"/>
+      <c r="K42" s="49"/>
     </row>
     <row r="43" spans="2:11">
       <c r="D43" s="3" t="s">
@@ -7634,7 +7634,7 @@
       <c r="J43" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="K43" s="51"/>
+      <c r="K43" s="50"/>
     </row>
     <row r="44" spans="2:11">
       <c r="B44" s="3" t="s">
@@ -7647,7 +7647,7 @@
         <v>28</v>
       </c>
       <c r="K44" s="33" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
     </row>
     <row r="45" spans="2:11">
@@ -7665,17 +7665,17 @@
       </c>
     </row>
     <row r="46" spans="2:11">
-      <c r="B46" s="47" t="s">
-        <v>328</v>
+      <c r="B46" s="46" t="s">
+        <v>325</v>
       </c>
       <c r="I46" s="4" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="J46" s="4" t="s">
         <v>28</v>
       </c>
       <c r="K46" s="33" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
     </row>
     <row r="47" spans="2:11">
@@ -7687,7 +7687,7 @@
       </c>
       <c r="J47" s="2"/>
       <c r="K47" s="33" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
     </row>
     <row r="48" spans="2:11">

</xml_diff>

<commit_message>
Mapped MedicationDispenseRequest to STU3
</commit_message>
<xml_diff>
--- a/Mappings/Medicatie9.xlsx
+++ b/Mappings/Medicatie9.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17726"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\Nictiz-STU3\Mappings\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7800" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7800" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="MedicatieAfspraak" sheetId="2" r:id="rId1"/>
@@ -24,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1448" uniqueCount="359">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1449" uniqueCount="361">
   <si>
     <t>1 … 1</t>
   </si>
@@ -959,9 +964,6 @@
     <t>MedicationAdministration.MedicationReference(Medication)</t>
   </si>
   <si>
-    <t>AfwijkendeToedining</t>
-  </si>
-  <si>
     <t xml:space="preserve">0….1 </t>
   </si>
   <si>
@@ -986,9 +988,6 @@
     <t>geannuleerd indicator</t>
   </si>
   <si>
-    <t xml:space="preserve">    AanvullendeInformatie</t>
-  </si>
-  <si>
     <t>Aanvullende Informatie</t>
   </si>
   <si>
@@ -1101,12 +1100,24 @@
   </si>
   <si>
     <t>Extension removed</t>
+  </si>
+  <si>
+    <t>AfwijkendeToediening</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MedicationAdministration.prescription(mp9-ToedieningsAfspraak) </t>
+  </si>
+  <si>
+    <t>Reference(mp9-ToedieningsAfspraak).identifier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    AanvullendeWensen</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="14">
     <font>
       <sz val="11"/>
@@ -1198,7 +1209,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1247,6 +1258,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1312,7 +1335,7 @@
     <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
@@ -1450,6 +1473,8 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -1780,7 +1805,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1790,7 +1815,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L88"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="G71" sqref="G71"/>
     </sheetView>
   </sheetViews>
@@ -2482,7 +2507,7 @@
         <v>52</v>
       </c>
       <c r="K52" s="21" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="53" spans="1:11">
@@ -2497,7 +2522,7 @@
         <v>52</v>
       </c>
       <c r="K53" s="21" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="54" spans="1:11">
@@ -2512,7 +2537,7 @@
         <v>52</v>
       </c>
       <c r="K54" s="21" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="55" spans="1:11">
@@ -4482,8 +4507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N78"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K78" sqref="K78"/>
+    <sheetView topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="2"/>
@@ -4707,16 +4732,16 @@
     </row>
     <row r="16" spans="1:14">
       <c r="B16" s="3" t="s">
+        <v>357</v>
+      </c>
+      <c r="I16" s="4" t="s">
         <v>311</v>
-      </c>
-      <c r="I16" s="4" t="s">
-        <v>312</v>
       </c>
       <c r="J16" s="4" t="s">
         <v>21</v>
       </c>
       <c r="K16" s="19" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="17" spans="2:14">
@@ -4781,16 +4806,16 @@
     </row>
     <row r="20" spans="2:14">
       <c r="B20" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="I20" s="4" t="s">
         <v>314</v>
-      </c>
-      <c r="I20" s="4" t="s">
-        <v>315</v>
       </c>
       <c r="J20" s="4" t="s">
         <v>21</v>
       </c>
       <c r="K20" s="34" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="M20" s="27"/>
       <c r="N20" s="27"/>
@@ -4824,7 +4849,7 @@
       </c>
       <c r="J22" s="2"/>
       <c r="K22" s="23" t="s">
-        <v>280</v>
+        <v>358</v>
       </c>
     </row>
     <row r="23" spans="2:14" s="38" customFormat="1">
@@ -4839,7 +4864,7 @@
         <v>17</v>
       </c>
       <c r="K23" s="43" t="s">
-        <v>281</v>
+        <v>359</v>
       </c>
     </row>
     <row r="24" spans="2:14">
@@ -4867,7 +4892,7 @@
       </c>
       <c r="J25" s="2"/>
       <c r="K25" s="25" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="26" spans="2:14" hidden="1" outlineLevel="1">
@@ -5078,7 +5103,7 @@
       </c>
       <c r="J43" s="2"/>
       <c r="K43" s="25" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="44" spans="3:11" hidden="1" outlineLevel="2">
@@ -5494,8 +5519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L77"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16:K31"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K76" sqref="K76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5559,7 +5584,7 @@
         <v>17</v>
       </c>
       <c r="K3" s="46" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -5620,7 +5645,7 @@
     </row>
     <row r="8" spans="1:12">
       <c r="B8" s="3" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="I8" s="4" t="s">
         <v>3</v>
@@ -5629,7 +5654,7 @@
         <v>21</v>
       </c>
       <c r="K8" s="46" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -5643,7 +5668,7 @@
         <v>8</v>
       </c>
       <c r="K9" s="46" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -5655,7 +5680,7 @@
       </c>
       <c r="J10" s="2"/>
       <c r="K10" s="46" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="L10" t="s">
         <v>205</v>
@@ -5670,7 +5695,7 @@
       </c>
       <c r="J11" s="2"/>
       <c r="K11" s="46" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -5717,7 +5742,7 @@
       <c r="J15" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="K15" t="s">
+      <c r="K15" s="54" t="s">
         <v>216</v>
       </c>
     </row>
@@ -5730,7 +5755,7 @@
       </c>
       <c r="J16" s="2"/>
       <c r="K16" s="26" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -5927,7 +5952,7 @@
       </c>
       <c r="J32" s="2"/>
       <c r="K32" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="33" spans="1:11">
@@ -5972,7 +5997,7 @@
         <v>4</v>
       </c>
       <c r="K35" s="18" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="36" spans="1:11">
@@ -6013,7 +6038,7 @@
         <v>52</v>
       </c>
       <c r="K38" s="35" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="39" spans="1:11">
@@ -6076,7 +6101,7 @@
         <v>52</v>
       </c>
       <c r="K43" s="21" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="44" spans="1:11">
@@ -6091,7 +6116,7 @@
         <v>52</v>
       </c>
       <c r="K44" s="21" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="45" spans="1:11">
@@ -6106,7 +6131,7 @@
         <v>52</v>
       </c>
       <c r="K45" s="21" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="46" spans="1:11">
@@ -6277,7 +6302,7 @@
         <v>8</v>
       </c>
       <c r="K57" s="10" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="58" spans="1:12">
@@ -6359,7 +6384,7 @@
       </c>
       <c r="J63" s="2"/>
       <c r="K63" s="36" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="64" spans="1:12">
@@ -6509,7 +6534,7 @@
     <row r="74" spans="1:12">
       <c r="A74" s="3"/>
       <c r="B74" s="46" t="s">
-        <v>320</v>
+        <v>360</v>
       </c>
       <c r="C74" s="46"/>
       <c r="D74" s="46"/>
@@ -6518,9 +6543,11 @@
       <c r="I74" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="J74" s="4"/>
-      <c r="K74" t="s">
-        <v>200</v>
+      <c r="J74" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="K74" s="53" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="75" spans="1:12">
@@ -6532,7 +6559,7 @@
         <v>22</v>
       </c>
       <c r="J75" s="4" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="K75" t="s">
         <v>200</v>
@@ -6558,7 +6585,7 @@
         <v>17</v>
       </c>
       <c r="K77" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="L77" t="s">
         <v>210</v>
@@ -6577,7 +6604,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="H1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
@@ -6633,7 +6660,7 @@
       </c>
       <c r="L2" s="27"/>
       <c r="M2" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -6680,7 +6707,7 @@
         <v>216</v>
       </c>
       <c r="L5" s="27" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="6" spans="1:13">
@@ -6695,7 +6722,7 @@
         <v>204</v>
       </c>
       <c r="L6" s="27" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -6707,10 +6734,10 @@
       </c>
       <c r="J7" s="2"/>
       <c r="K7" s="25" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="L7" s="27" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -7033,10 +7060,10 @@
     </row>
     <row r="32" spans="2:12">
       <c r="B32" s="3" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="J32" s="4" t="s">
         <v>4</v>
@@ -7188,7 +7215,7 @@
       </c>
       <c r="J5" s="2"/>
       <c r="K5" s="25" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="6" spans="1:12" hidden="1" outlineLevel="1">
@@ -7312,7 +7339,7 @@
       </c>
       <c r="J16" s="2"/>
       <c r="K16" s="25" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="17" spans="2:11">
@@ -7326,7 +7353,7 @@
         <v>31</v>
       </c>
       <c r="K17" s="25" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="18" spans="2:11">
@@ -7340,7 +7367,7 @@
         <v>8</v>
       </c>
       <c r="K18" s="25" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="19" spans="2:11">
@@ -7354,7 +7381,7 @@
         <v>52</v>
       </c>
       <c r="K19" s="25" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="20" spans="2:11">
@@ -7366,7 +7393,7 @@
       </c>
       <c r="J20" s="2"/>
       <c r="K20" s="26" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="21" spans="2:11">
@@ -7574,7 +7601,7 @@
         <v>19</v>
       </c>
       <c r="K37" s="25" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="38" spans="2:11">
@@ -7588,7 +7615,7 @@
         <v>149</v>
       </c>
       <c r="K38" s="25" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="39" spans="2:11">
@@ -7602,7 +7629,7 @@
         <v>19</v>
       </c>
       <c r="K39" s="25" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="40" spans="2:11">
@@ -7614,7 +7641,7 @@
       </c>
       <c r="J40" s="2"/>
       <c r="K40" s="51" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="41" spans="2:11">
@@ -7662,7 +7689,7 @@
         <v>28</v>
       </c>
       <c r="K44" s="33" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="45" spans="2:11">
@@ -7681,16 +7708,16 @@
     </row>
     <row r="46" spans="2:11">
       <c r="B46" s="46" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="I46" s="4" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="J46" s="4" t="s">
         <v>28</v>
       </c>
       <c r="K46" s="33" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="47" spans="2:11">
@@ -7702,7 +7729,7 @@
       </c>
       <c r="J47" s="2"/>
       <c r="K47" s="33" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="48" spans="2:11">

</xml_diff>

<commit_message>
Added Progress xlsx and Medication mapping xlsx
</commit_message>
<xml_diff>
--- a/Mappings/Medicatie9.xlsx
+++ b/Mappings/Medicatie9.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17726"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\Nictiz-STU3\Mappings\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7800" activeTab="3"/>
   </bookViews>
@@ -19,7 +14,7 @@
     <sheet name="Verstrekking" sheetId="6" r:id="rId5"/>
     <sheet name="Verstrekkingsverzoek" sheetId="7" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="145621" iterate="1"/>
+  <calcPr calcId="145621" iterate="1" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1449" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1468" uniqueCount="377">
   <si>
     <t>1 … 1</t>
   </si>
@@ -1112,12 +1107,60 @@
   </si>
   <si>
     <t xml:space="preserve">    AanvullendeWensen</t>
+  </si>
+  <si>
+    <t>??? Not sure - new</t>
+  </si>
+  <si>
+    <t>MedicationStatement.status</t>
+  </si>
+  <si>
+    <t>mapping ID: 22505</t>
+  </si>
+  <si>
+    <t>ID 22695</t>
+  </si>
+  <si>
+    <t>ID 22696</t>
+  </si>
+  <si>
+    <t>ID 22697</t>
+  </si>
+  <si>
+    <t>ID 22502</t>
+  </si>
+  <si>
+    <t>ID staan in geen enkel profiel</t>
+  </si>
+  <si>
+    <t>ID 22618</t>
+  </si>
+  <si>
+    <t>Kan dit niet vinden</t>
+  </si>
+  <si>
+    <t>22508 </t>
+  </si>
+  <si>
+    <t>Moet deze valueset niet gekoppeld worden? http://decor.nictiz.nl/medicatieproces/mp-html-20170601T173502/voc-2.16.840.1.113883.2.4.3.11.60.20.77.11.35-2017-05-09T103908.html</t>
+  </si>
+  <si>
+    <t>Zou mooi zijn als we dit nog wel verder zouden kunnen specificiren vind je niet?</t>
+  </si>
+  <si>
+    <t>zit nu op .basedOn wat volgens mij correct is.</t>
+  </si>
+  <si>
+    <t>Why binding on required?</t>
+  </si>
+  <si>
+    <t>Is momenteel niet verplicht in het profiel.  Of is dit gewoon het technische ID? Hij staat iig op identifier gemapt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="14">
     <font>
       <sz val="11"/>
@@ -1335,7 +1378,7 @@
     <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
@@ -1470,11 +1513,15 @@
     <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="2" applyAlignment="1">
+      <alignment vertical="top" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -1805,7 +1852,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1815,8 +1862,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L88"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G71" sqref="G71"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1"/>
@@ -1833,16 +1880,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="54" t="s">
         <v>152</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
       <c r="I1" s="1" t="s">
         <v>132</v>
       </c>
@@ -3015,10 +3062,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L115"/>
+  <dimension ref="A1:L116"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="4"/>
@@ -3032,20 +3079,20 @@
     <col min="8" max="8" width="17.42578125" customWidth="1"/>
     <col min="10" max="10" width="12" customWidth="1"/>
     <col min="11" max="11" width="57" style="11" customWidth="1"/>
-    <col min="12" max="12" width="61.7109375" customWidth="1"/>
+    <col min="12" max="12" width="166.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="54" t="s">
         <v>152</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
       <c r="I1" s="1" t="s">
         <v>132</v>
       </c>
@@ -3131,387 +3178,400 @@
       </c>
     </row>
     <row r="7" spans="1:12">
-      <c r="B7" s="3" t="s">
-        <v>29</v>
+      <c r="B7" s="56" t="s">
+        <v>97</v>
       </c>
       <c r="I7" s="4" t="s">
         <v>3</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="K7" s="10" t="s">
-        <v>156</v>
+        <v>8</v>
+      </c>
+      <c r="K7" s="39" t="s">
+        <v>362</v>
+      </c>
+      <c r="L7" t="s">
+        <v>361</v>
       </c>
     </row>
     <row r="8" spans="1:12">
       <c r="B8" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I8" s="4" t="s">
         <v>3</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="K8" s="10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="B9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="K9" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="L9" s="55"/>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="B10" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="I9" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="J9" s="4" t="s">
+      <c r="I10" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J10" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="K9" s="10" t="s">
+      <c r="K10" s="10" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
-      <c r="A10" s="5" t="s">
+    <row r="11" spans="1:12">
+      <c r="A11" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="I10" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="J10" s="2"/>
-      <c r="K10" s="26" t="s">
+      <c r="I11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J11" s="2"/>
+      <c r="K11" s="26" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
-      <c r="B11" s="3" t="s">
+    <row r="12" spans="1:12">
+      <c r="B12" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="I11" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="J11" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="K11" s="18" t="s">
+      <c r="I12" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="K12" s="18" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
-      <c r="B12" s="5" t="s">
+    <row r="13" spans="1:12">
+      <c r="B13" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="I12" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-    </row>
-    <row r="13" spans="1:12">
-      <c r="C13" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="I13" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="J13" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="K13" s="18" t="s">
-        <v>159</v>
-      </c>
+      <c r="I13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
     </row>
     <row r="14" spans="1:12">
       <c r="C14" s="3" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J14" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="K14" s="22" t="s">
-        <v>160</v>
+      <c r="K14" s="18" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="15" spans="1:12">
       <c r="C15" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="K15" s="22" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="C16" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="I15" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="J15" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="K15" s="18" t="s">
+      <c r="I16" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="K16" s="18" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
-      <c r="B16" s="5" t="s">
+    <row r="17" spans="1:12">
+      <c r="B17" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="I16" s="2" t="s">
+      <c r="I17" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="J16" s="2"/>
-      <c r="K16" s="18" t="s">
+      <c r="J17" s="2"/>
+      <c r="K17" s="18" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
-      <c r="C17" s="5" t="s">
+    <row r="18" spans="1:12">
+      <c r="C18" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="I17" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-    </row>
-    <row r="18" spans="1:11">
-      <c r="D18" s="5" t="s">
+      <c r="I18" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="D19" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="I18" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="J18" s="2"/>
-      <c r="K18" s="18" t="s">
+      <c r="I19" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J19" s="2"/>
+      <c r="K19" s="18" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
-      <c r="E19" s="3" t="s">
+    <row r="20" spans="1:12">
+      <c r="E20" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="I19" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="J19" s="4" t="s">
+      <c r="I20" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="J20" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="K19" s="18"/>
-    </row>
-    <row r="20" spans="1:11">
-      <c r="E20" s="3" t="s">
+      <c r="K20" s="18"/>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="E21" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="I20" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="J20" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="K20" s="18"/>
-    </row>
-    <row r="21" spans="1:11">
-      <c r="D21" s="5" t="s">
+      <c r="I21" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="K21" s="18"/>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="D22" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="I21" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="J21" s="2"/>
-      <c r="K21" s="10" t="s">
+      <c r="I22" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J22" s="2"/>
+      <c r="K22" s="10" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
-      <c r="E22" s="3" t="s">
+    <row r="23" spans="1:12">
+      <c r="E23" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="I22" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="J22" s="4" t="s">
+      <c r="I23" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="J23" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="K22" s="10"/>
-    </row>
-    <row r="23" spans="1:11">
-      <c r="E23" s="3" t="s">
+      <c r="K23" s="10"/>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="E24" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="I23" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="J23" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="K23" s="10"/>
-    </row>
-    <row r="24" spans="1:11">
-      <c r="B24" s="3" t="s">
+      <c r="I24" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="J24" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="K24" s="10"/>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="B25" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D24" s="3"/>
-      <c r="I24" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="J24" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="K24" s="18" t="s">
+      <c r="D25" s="3"/>
+      <c r="I25" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J25" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="K25" s="18" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
-      <c r="A25" s="5" t="s">
+    <row r="26" spans="1:12">
+      <c r="A26" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="I25" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="J25" s="2"/>
-      <c r="K25" t="s">
+      <c r="I26" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J26" s="2"/>
+      <c r="K26" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
-      <c r="B26" s="3" t="s">
+    <row r="27" spans="1:12">
+      <c r="B27" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="I26" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="J26" s="4" t="s">
+      <c r="I27" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="J27" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="K26" s="18" t="s">
+      <c r="K27" s="18" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
-      <c r="B27" s="3" t="s">
+    <row r="28" spans="1:12">
+      <c r="B28" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="I27" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="J27" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="K27" s="18" t="s">
+      <c r="I28" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J28" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="K28" s="18" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="28" spans="1:11">
-      <c r="B28" s="3" t="s">
+    <row r="29" spans="1:12">
+      <c r="B29" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="I28" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="J28" s="4" t="s">
+      <c r="I29" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J29" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="K28" s="18" t="s">
+      <c r="K29" s="18" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
-      <c r="B29" s="3" t="s">
+    <row r="30" spans="1:12">
+      <c r="B30" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="I29" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="J29" s="4" t="s">
+      <c r="I30" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J30" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="K29" s="10" t="s">
+      <c r="K30" s="10" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="30" spans="1:11">
-      <c r="B30" s="5" t="s">
+      <c r="L30" s="55" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
+      <c r="B31" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="I30" s="2" t="s">
+      <c r="I31" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="J30" s="2"/>
-      <c r="K30" s="2"/>
-    </row>
-    <row r="31" spans="1:11">
-      <c r="C31" s="3" t="s">
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+    </row>
+    <row r="32" spans="1:12">
+      <c r="C32" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="I31" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="J31" s="4" t="s">
+      <c r="I32" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J32" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="K31" s="35" t="s">
+      <c r="K32" s="35" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="32" spans="1:11">
-      <c r="C32" s="3" t="s">
+    <row r="33" spans="3:12">
+      <c r="C33" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="I32" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="J32" s="4" t="s">
+      <c r="I33" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J33" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="K32" s="10" t="s">
+      <c r="K33" s="10" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="33" spans="3:11">
-      <c r="C33" s="5" t="s">
+    <row r="34" spans="3:12">
+      <c r="C34" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="I33" s="2" t="s">
+      <c r="I34" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="J33" s="2"/>
-      <c r="K33" s="2"/>
-    </row>
-    <row r="34" spans="3:11">
-      <c r="D34" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="I34" s="2" t="s">
-        <v>3</v>
       </c>
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
     </row>
-    <row r="35" spans="3:11">
-      <c r="E35" s="5" t="s">
-        <v>55</v>
+    <row r="35" spans="3:12">
+      <c r="D35" s="5" t="s">
+        <v>54</v>
       </c>
       <c r="I35" s="2" t="s">
         <v>3</v>
       </c>
       <c r="J35" s="2"/>
       <c r="K35" s="2"/>
-    </row>
-    <row r="36" spans="3:11">
-      <c r="F36" s="3" t="s">
+      <c r="L35" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="36" spans="3:12">
+      <c r="E36" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="55" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="37" spans="3:12">
+      <c r="F37" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="I36" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="J36" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="K36" s="21" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="37" spans="3:11">
-      <c r="F37" s="3" t="s">
-        <v>57</v>
       </c>
       <c r="I37" s="4" t="s">
         <v>3</v>
@@ -3520,12 +3580,15 @@
         <v>52</v>
       </c>
       <c r="K37" s="21" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="38" spans="3:11">
+        <v>292</v>
+      </c>
+      <c r="L37" s="55" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="38" spans="3:12">
       <c r="F38" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I38" s="4" t="s">
         <v>3</v>
@@ -3534,50 +3597,66 @@
         <v>52</v>
       </c>
       <c r="K38" s="21" t="s">
+        <v>293</v>
+      </c>
+      <c r="L38" s="55" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="39" spans="3:12">
+      <c r="F39" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="I39" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J39" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="K39" s="21" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="39" spans="3:11">
-      <c r="F39" s="3" t="s">
+      <c r="L39" s="55" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="40" spans="3:12">
+      <c r="F40" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="I39" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="J39" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="K39" s="11" t="s">
+      <c r="I40" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J40" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="K40" s="11" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="40" spans="3:11">
-      <c r="F40" s="3" t="s">
+      <c r="L40" s="55" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="41" spans="3:12">
+      <c r="F41" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="I40" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="J40" s="4" t="s">
+      <c r="I41" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J41" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="K40" s="21" t="s">
+      <c r="K41" s="21" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="41" spans="3:11">
-      <c r="D41" s="5" t="s">
+      <c r="L41" s="55" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="42" spans="3:12">
+      <c r="D42" s="5" t="s">
         <v>60</v>
-      </c>
-      <c r="I41" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="J41" s="2"/>
-      <c r="K41" s="2"/>
-    </row>
-    <row r="42" spans="3:11">
-      <c r="E42" s="5" t="s">
-        <v>61</v>
       </c>
       <c r="I42" s="2" t="s">
         <v>3</v>
@@ -3585,9 +3664,9 @@
       <c r="J42" s="2"/>
       <c r="K42" s="2"/>
     </row>
-    <row r="43" spans="3:11">
-      <c r="F43" s="5" t="s">
-        <v>55</v>
+    <row r="43" spans="3:12">
+      <c r="E43" s="5" t="s">
+        <v>61</v>
       </c>
       <c r="I43" s="2" t="s">
         <v>3</v>
@@ -3595,23 +3674,19 @@
       <c r="J43" s="2"/>
       <c r="K43" s="2"/>
     </row>
-    <row r="44" spans="3:11">
-      <c r="G44" s="3" t="s">
+    <row r="44" spans="3:12">
+      <c r="F44" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="I44" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J44" s="2"/>
+      <c r="K44" s="2"/>
+    </row>
+    <row r="45" spans="3:12">
+      <c r="G45" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="I44" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="J44" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="K44" s="10" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="45" spans="3:11">
-      <c r="G45" s="3" t="s">
-        <v>57</v>
       </c>
       <c r="I45" s="4" t="s">
         <v>3</v>
@@ -3623,9 +3698,9 @@
         <v>295</v>
       </c>
     </row>
-    <row r="46" spans="3:11">
+    <row r="46" spans="3:12">
       <c r="G46" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I46" s="4" t="s">
         <v>3</v>
@@ -3634,222 +3709,228 @@
         <v>52</v>
       </c>
       <c r="K46" s="10" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="47" spans="3:12">
+      <c r="G47" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="I47" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J47" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="K47" s="10" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="47" spans="3:11">
-      <c r="F47" s="3" t="s">
+    <row r="48" spans="3:12">
+      <c r="F48" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="I47" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="J47" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="K47" s="10" t="s">
+      <c r="I48" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J48" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="K48" s="10" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="48" spans="3:11">
-      <c r="E48" s="3" t="s">
+      <c r="L48" s="55" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="49" spans="5:12">
+      <c r="E49" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="I48" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="J48" s="4" t="s">
+      <c r="I49" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J49" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="K48" s="10" t="s">
+      <c r="K49" s="10" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="49" spans="5:11">
-      <c r="E49" s="3" t="s">
+    <row r="50" spans="5:12">
+      <c r="E50" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="I49" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="J49" s="4" t="s">
+      <c r="I50" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J50" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="K49" s="10" t="s">
+      <c r="K50" s="10" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="50" spans="5:11">
-      <c r="E50" s="3" t="s">
+    <row r="51" spans="5:12">
+      <c r="E51" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="I50" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="J50" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="K50" s="10" t="s">
+      <c r="I51" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J51" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="K51" s="10" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="51" spans="5:11">
-      <c r="E51" s="3" t="s">
+    <row r="52" spans="5:12">
+      <c r="E52" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="I51" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="J51" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="K51" s="35" t="s">
+      <c r="I52" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J52" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="K52" s="35" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="52" spans="5:11">
-      <c r="E52" s="5" t="s">
+    <row r="53" spans="5:12">
+      <c r="E53" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="I52" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="J52" s="2"/>
-      <c r="K52" s="18" t="s">
+      <c r="I53" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J53" s="2"/>
+      <c r="K53" s="18" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="53" spans="5:11">
-      <c r="F53" s="5" t="s">
+    <row r="54" spans="5:12">
+      <c r="F54" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="I53" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="J53" s="2"/>
-      <c r="K53" s="2"/>
-    </row>
-    <row r="54" spans="5:11">
-      <c r="G54" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I54" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="J54" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="K54" s="18" t="s">
+      <c r="I54" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J54" s="2"/>
+      <c r="K54" s="2"/>
+    </row>
+    <row r="55" spans="5:12">
+      <c r="G55" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I55" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J55" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="K55" s="18" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="55" spans="5:11">
-      <c r="G55" s="3" t="s">
+      <c r="L55" s="55" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="56" spans="5:12">
+      <c r="G56" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="I55" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="J55" s="4" t="s">
+      <c r="I56" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J56" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="K55" s="18" t="s">
+      <c r="K56" s="18" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="56" spans="5:11">
-      <c r="F56" s="5" t="s">
+    <row r="57" spans="5:12">
+      <c r="F57" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="I56" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="J56" s="2"/>
-      <c r="K56" s="36" t="s">
+      <c r="I57" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J57" s="2"/>
+      <c r="K57" s="36" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="57" spans="5:11">
-      <c r="G57" s="3" t="s">
+    <row r="58" spans="5:12">
+      <c r="G58" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="I57" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="J57" s="4" t="s">
+      <c r="I58" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J58" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="K57" s="10" t="s">
+      <c r="K58" s="10" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="58" spans="5:11">
-      <c r="G58" s="3" t="s">
+    <row r="59" spans="5:12">
+      <c r="G59" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="I58" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="J58" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="K58" s="10" t="s">
+      <c r="I59" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J59" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="K59" s="10" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="59" spans="5:11">
-      <c r="G59" s="3" t="s">
+    <row r="60" spans="5:12">
+      <c r="G60" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="I59" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="J59" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="K59" s="10" t="s">
+      <c r="I60" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J60" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="K60" s="10" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="60" spans="5:11">
-      <c r="E60" s="5" t="s">
+    <row r="61" spans="5:12">
+      <c r="E61" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="I60" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="J60" s="2"/>
-      <c r="K60" s="10" t="s">
+      <c r="I61" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J61" s="2"/>
+      <c r="K61" s="10" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="61" spans="5:11">
-      <c r="F61" s="5" t="s">
+    <row r="62" spans="5:12">
+      <c r="F62" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="I61" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="J61" s="2"/>
-      <c r="K61" s="2"/>
-    </row>
-    <row r="62" spans="5:11">
-      <c r="G62" s="3" t="s">
+      <c r="I62" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J62" s="2"/>
+      <c r="K62" s="2"/>
+    </row>
+    <row r="63" spans="5:12">
+      <c r="G63" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="I62" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="J62" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="K62" s="10" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="63" spans="5:11">
-      <c r="G63" s="3" t="s">
-        <v>57</v>
       </c>
       <c r="I63" s="4" t="s">
         <v>3</v>
@@ -3858,12 +3939,12 @@
         <v>52</v>
       </c>
       <c r="K63" s="10" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="64" spans="5:11">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="64" spans="5:12">
       <c r="G64" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I64" s="4" t="s">
         <v>3</v>
@@ -3872,26 +3953,29 @@
         <v>52</v>
       </c>
       <c r="K64" s="10" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="65" spans="2:12">
+      <c r="G65" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="I65" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J65" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="K65" s="10" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="65" spans="2:11">
-      <c r="F65" s="3" t="s">
+      <c r="L65" s="17" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="66" spans="2:12">
+      <c r="F66" s="3" t="s">
         <v>43</v>
-      </c>
-      <c r="I65" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="J65" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="K65" s="10" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="66" spans="2:11">
-      <c r="F66" s="3" t="s">
-        <v>62</v>
       </c>
       <c r="I66" s="4" t="s">
         <v>3</v>
@@ -3903,107 +3987,112 @@
         <v>163</v>
       </c>
     </row>
-    <row r="67" spans="2:11">
-      <c r="B67" s="5" t="s">
+    <row r="67" spans="2:12">
+      <c r="F67" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="I67" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J67" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="K67" s="10" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="68" spans="2:12">
+      <c r="B68" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="I67" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="J67" s="2"/>
-      <c r="K67" s="23" t="s">
+      <c r="I68" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J68" s="2"/>
+      <c r="K68" s="23" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="68" spans="2:11" s="38" customFormat="1">
-      <c r="B68" s="41"/>
-      <c r="C68" s="41" t="s">
+      <c r="L68" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="69" spans="2:12" s="38" customFormat="1">
+      <c r="B69" s="41"/>
+      <c r="C69" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="I68" s="42" t="s">
-        <v>3</v>
-      </c>
-      <c r="J68" s="42" t="s">
+      <c r="I69" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="J69" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="K68" s="43" t="s">
+      <c r="K69" s="43" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="69" spans="2:11">
-      <c r="B69" s="5" t="s">
+    <row r="70" spans="2:12">
+      <c r="B70" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="I69" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="J69" s="2"/>
-      <c r="K69" s="23" t="s">
+      <c r="I70" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J70" s="2"/>
+      <c r="K70" s="23" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="70" spans="2:11" s="38" customFormat="1">
-      <c r="B70" s="41"/>
-      <c r="C70" s="41" t="s">
+    <row r="71" spans="2:12" s="38" customFormat="1">
+      <c r="B71" s="41"/>
+      <c r="C71" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="I70" s="42" t="s">
-        <v>3</v>
-      </c>
-      <c r="J70" s="42" t="s">
+      <c r="I71" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="J71" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="K70" s="43" t="s">
+      <c r="K71" s="43" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="71" spans="2:11" s="38" customFormat="1">
-      <c r="B71" s="38" t="s">
+    <row r="72" spans="2:12" s="38" customFormat="1">
+      <c r="B72" s="38" t="s">
         <v>73</v>
       </c>
-      <c r="I71" s="42" t="s">
-        <v>3</v>
-      </c>
-      <c r="J71" s="42"/>
-      <c r="K71" s="43" t="s">
+      <c r="I72" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="J72" s="42"/>
+      <c r="K72" s="43" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="72" spans="2:11" hidden="1" outlineLevel="2">
-      <c r="B72" s="5" t="s">
+    <row r="73" spans="2:12" hidden="1" outlineLevel="2">
+      <c r="B73" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="I72" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="J72" s="2"/>
-      <c r="K72" s="10"/>
-    </row>
-    <row r="73" spans="2:11" hidden="1" outlineLevel="2">
-      <c r="C73" s="5" t="s">
-        <v>1</v>
-      </c>
       <c r="I73" s="2" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J73" s="2"/>
       <c r="K73" s="10"/>
     </row>
-    <row r="74" spans="2:11" hidden="1" outlineLevel="2">
-      <c r="D74" s="3" t="s">
+    <row r="74" spans="2:12" hidden="1" outlineLevel="2">
+      <c r="C74" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I74" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J74" s="2"/>
+      <c r="K74" s="10"/>
+    </row>
+    <row r="75" spans="2:12" hidden="1" outlineLevel="2">
+      <c r="D75" s="3" t="s">
         <v>2</v>
-      </c>
-      <c r="I74" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="J74" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="K74" s="10"/>
-    </row>
-    <row r="75" spans="2:11" hidden="1" outlineLevel="2">
-      <c r="D75" s="3" t="s">
-        <v>5</v>
       </c>
       <c r="I75" s="4" t="s">
         <v>3</v>
@@ -4013,118 +4102,120 @@
       </c>
       <c r="K75" s="10"/>
     </row>
-    <row r="76" spans="2:11" hidden="1" outlineLevel="2">
-      <c r="C76" s="5" t="s">
+    <row r="76" spans="2:12" hidden="1" outlineLevel="2">
+      <c r="D76" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I76" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J76" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="K76" s="10"/>
+    </row>
+    <row r="77" spans="2:12" hidden="1" outlineLevel="2">
+      <c r="C77" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="I76" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="J76" s="2"/>
-      <c r="K76" s="10"/>
-    </row>
-    <row r="77" spans="2:11" hidden="1" outlineLevel="2">
-      <c r="D77" s="3" t="s">
+      <c r="I77" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J77" s="2"/>
+      <c r="K77" s="10"/>
+    </row>
+    <row r="78" spans="2:12" hidden="1" outlineLevel="2">
+      <c r="D78" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="I77" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="J77" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="K77" s="10"/>
-    </row>
-    <row r="78" spans="2:11" hidden="1" outlineLevel="2">
-      <c r="D78" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="I78" s="4" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J78" s="4" t="s">
         <v>4</v>
       </c>
       <c r="K78" s="10"/>
     </row>
-    <row r="79" spans="2:11" hidden="1" outlineLevel="2">
-      <c r="C79" s="3" t="s">
+    <row r="79" spans="2:12" hidden="1" outlineLevel="2">
+      <c r="D79" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I79" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="J79" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="K79" s="10"/>
+    </row>
+    <row r="80" spans="2:12" hidden="1" outlineLevel="2">
+      <c r="C80" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="I79" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="J79" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="K79" s="10"/>
-    </row>
-    <row r="80" spans="2:11" hidden="1" outlineLevel="2">
-      <c r="B80" s="3" t="s">
+      <c r="I80" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J80" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="K80" s="10"/>
+    </row>
+    <row r="81" spans="1:11" hidden="1" outlineLevel="2">
+      <c r="B81" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="I80" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="J80" s="4" t="s">
+      <c r="I81" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J81" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="K80" s="10"/>
-    </row>
-    <row r="81" spans="1:11" hidden="1" outlineLevel="2">
-      <c r="B81" s="5" t="s">
+      <c r="K81" s="10"/>
+    </row>
+    <row r="82" spans="1:11" hidden="1" outlineLevel="2">
+      <c r="B82" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="I81" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="J81" s="2"/>
-      <c r="K81" s="10"/>
-    </row>
-    <row r="82" spans="1:11" hidden="1" outlineLevel="2">
-      <c r="A82" s="13"/>
-      <c r="B82" s="13"/>
-      <c r="C82" s="13" t="s">
+      <c r="I82" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J82" s="2"/>
+      <c r="K82" s="10"/>
+    </row>
+    <row r="83" spans="1:11" hidden="1" outlineLevel="2">
+      <c r="A83" s="13"/>
+      <c r="B83" s="13"/>
+      <c r="C83" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="D82" s="13"/>
-      <c r="E82" s="13"/>
-      <c r="F82" s="13"/>
-      <c r="G82" s="13"/>
-      <c r="H82" s="13"/>
-      <c r="I82" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="J82" s="14"/>
-      <c r="K82" s="20" t="s">
+      <c r="D83" s="13"/>
+      <c r="E83" s="13"/>
+      <c r="F83" s="13"/>
+      <c r="G83" s="13"/>
+      <c r="H83" s="13"/>
+      <c r="I83" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="J83" s="14"/>
+      <c r="K83" s="20" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="83" spans="1:11" hidden="1" outlineLevel="4">
-      <c r="D83" s="3" t="s">
+    <row r="84" spans="1:11" hidden="1" outlineLevel="4">
+      <c r="D84" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="I83" s="4" t="s">
+      <c r="I84" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="J83" s="4" t="s">
+      <c r="J84" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="K83" s="20"/>
-    </row>
-    <row r="84" spans="1:11" hidden="1" outlineLevel="4">
-      <c r="D84" s="5" t="s">
+      <c r="K84" s="20"/>
+    </row>
+    <row r="85" spans="1:11" hidden="1" outlineLevel="4">
+      <c r="D85" s="5" t="s">
         <v>80</v>
-      </c>
-      <c r="I84" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="J84" s="2"/>
-      <c r="K84" s="20"/>
-    </row>
-    <row r="85" spans="1:11" hidden="1" outlineLevel="4">
-      <c r="E85" s="5" t="s">
-        <v>1</v>
       </c>
       <c r="I85" s="2" t="s">
         <v>0</v>
@@ -4133,20 +4224,18 @@
       <c r="K85" s="20"/>
     </row>
     <row r="86" spans="1:11" hidden="1" outlineLevel="4">
-      <c r="F86" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I86" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="J86" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="E86" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I86" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J86" s="2"/>
       <c r="K86" s="20"/>
     </row>
     <row r="87" spans="1:11" hidden="1" outlineLevel="4">
       <c r="F87" s="3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I87" s="4" t="s">
         <v>3</v>
@@ -4157,33 +4246,33 @@
       <c r="K87" s="20"/>
     </row>
     <row r="88" spans="1:11" hidden="1" outlineLevel="4">
-      <c r="E88" s="5" t="s">
+      <c r="F88" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I88" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J88" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="K88" s="20"/>
+    </row>
+    <row r="89" spans="1:11" hidden="1" outlineLevel="4">
+      <c r="E89" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="I88" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="J88" s="2"/>
-      <c r="K88" s="20"/>
-    </row>
-    <row r="89" spans="1:11" hidden="1" outlineLevel="4">
-      <c r="F89" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I89" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="J89" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="I89" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J89" s="2"/>
       <c r="K89" s="20"/>
     </row>
     <row r="90" spans="1:11" hidden="1" outlineLevel="4">
       <c r="F90" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I90" s="4" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J90" s="4" t="s">
         <v>4</v>
@@ -4191,30 +4280,32 @@
       <c r="K90" s="20"/>
     </row>
     <row r="91" spans="1:11" hidden="1" outlineLevel="4">
-      <c r="D91" s="3" t="s">
+      <c r="F91" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I91" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="J91" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="K91" s="20"/>
+    </row>
+    <row r="92" spans="1:11" hidden="1" outlineLevel="4">
+      <c r="D92" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="F91" s="3"/>
-      <c r="I91" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="J91" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="K91" s="20"/>
-    </row>
-    <row r="92" spans="1:11" hidden="1" outlineLevel="4">
-      <c r="D92" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="I92" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="J92" s="2"/>
+      <c r="F92" s="3"/>
+      <c r="I92" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J92" s="4" t="s">
+        <v>8</v>
+      </c>
       <c r="K92" s="20"/>
     </row>
     <row r="93" spans="1:11" hidden="1" outlineLevel="4">
-      <c r="E93" s="5" t="s">
+      <c r="D93" s="5" t="s">
         <v>82</v>
       </c>
       <c r="I93" s="2" t="s">
@@ -4224,105 +4315,105 @@
       <c r="K93" s="20"/>
     </row>
     <row r="94" spans="1:11" hidden="1" outlineLevel="4">
-      <c r="F94" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="I94" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J94" s="4" t="s">
-        <v>17</v>
-      </c>
+      <c r="E94" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="I94" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J94" s="2"/>
       <c r="K94" s="20"/>
     </row>
     <row r="95" spans="1:11" hidden="1" outlineLevel="4">
       <c r="F95" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="I95" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J95" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K95" s="20"/>
+    </row>
+    <row r="96" spans="1:11" hidden="1" outlineLevel="4">
+      <c r="F96" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="I95" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="J95" s="4" t="s">
+      <c r="I96" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="J96" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="K95" s="20"/>
-    </row>
-    <row r="96" spans="1:11" hidden="1" outlineLevel="2">
-      <c r="A96" s="15"/>
-      <c r="B96" s="15" t="s">
+      <c r="K96" s="20"/>
+    </row>
+    <row r="97" spans="1:11" hidden="1" outlineLevel="2">
+      <c r="A97" s="15"/>
+      <c r="B97" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="C96" s="15"/>
-      <c r="D96" s="15"/>
-      <c r="E96" s="15"/>
-      <c r="F96" s="15"/>
-      <c r="G96" s="15"/>
-      <c r="H96" s="15"/>
-      <c r="I96" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="J96" s="16"/>
-      <c r="K96" s="20" t="s">
+      <c r="C97" s="15"/>
+      <c r="D97" s="15"/>
+      <c r="E97" s="15"/>
+      <c r="F97" s="15"/>
+      <c r="G97" s="15"/>
+      <c r="H97" s="15"/>
+      <c r="I97" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="J97" s="16"/>
+      <c r="K97" s="20" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="97" spans="3:11" hidden="1" outlineLevel="3">
-      <c r="C97" s="3" t="s">
+    <row r="98" spans="1:11" hidden="1" outlineLevel="3">
+      <c r="C98" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="I97" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="J97" s="4" t="s">
+      <c r="I98" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J98" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="K97" s="10"/>
-    </row>
-    <row r="98" spans="3:11" hidden="1" outlineLevel="3">
-      <c r="C98" s="5" t="s">
+      <c r="K98" s="10"/>
+    </row>
+    <row r="99" spans="1:11" hidden="1" outlineLevel="3">
+      <c r="C99" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="I98" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="J98" s="2"/>
-      <c r="K98" s="10"/>
-    </row>
-    <row r="99" spans="3:11" hidden="1" outlineLevel="3">
-      <c r="D99" s="5" t="s">
-        <v>78</v>
-      </c>
       <c r="I99" s="2" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J99" s="2"/>
       <c r="K99" s="10"/>
     </row>
-    <row r="100" spans="3:11" hidden="1" outlineLevel="3">
-      <c r="E100" s="3" t="s">
+    <row r="100" spans="1:11" hidden="1" outlineLevel="3">
+      <c r="D100" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="I100" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J100" s="2"/>
+      <c r="K100" s="10"/>
+    </row>
+    <row r="101" spans="1:11" hidden="1" outlineLevel="3">
+      <c r="E101" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="I100" s="4" t="s">
+      <c r="I101" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="J100" s="4" t="s">
+      <c r="J101" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="K100" s="10"/>
-    </row>
-    <row r="101" spans="3:11" hidden="1" outlineLevel="3">
-      <c r="E101" s="5" t="s">
+      <c r="K101" s="10"/>
+    </row>
+    <row r="102" spans="1:11" hidden="1" outlineLevel="3">
+      <c r="E102" s="5" t="s">
         <v>80</v>
-      </c>
-      <c r="I101" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="J101" s="2"/>
-      <c r="K101" s="10"/>
-    </row>
-    <row r="102" spans="3:11" hidden="1" outlineLevel="3">
-      <c r="F102" s="5" t="s">
-        <v>1</v>
       </c>
       <c r="I102" s="2" t="s">
         <v>0</v>
@@ -4330,21 +4421,19 @@
       <c r="J102" s="2"/>
       <c r="K102" s="10"/>
     </row>
-    <row r="103" spans="3:11" hidden="1" outlineLevel="3">
-      <c r="G103" s="3" t="s">
+    <row r="103" spans="1:11" hidden="1" outlineLevel="3">
+      <c r="F103" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I103" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J103" s="2"/>
+      <c r="K103" s="10"/>
+    </row>
+    <row r="104" spans="1:11" hidden="1" outlineLevel="3">
+      <c r="G104" s="3" t="s">
         <v>2</v>
-      </c>
-      <c r="I103" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="J103" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="K103" s="10"/>
-    </row>
-    <row r="104" spans="3:11" hidden="1" outlineLevel="3">
-      <c r="G104" s="3" t="s">
-        <v>5</v>
       </c>
       <c r="I104" s="4" t="s">
         <v>3</v>
@@ -4354,65 +4443,67 @@
       </c>
       <c r="K104" s="10"/>
     </row>
-    <row r="105" spans="3:11" hidden="1" outlineLevel="3">
-      <c r="F105" s="5" t="s">
+    <row r="105" spans="1:11" hidden="1" outlineLevel="3">
+      <c r="G105" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I105" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J105" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="K105" s="10"/>
+    </row>
+    <row r="106" spans="1:11" hidden="1" outlineLevel="3">
+      <c r="F106" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="I105" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="J105" s="2"/>
-      <c r="K105" s="10"/>
-    </row>
-    <row r="106" spans="3:11" hidden="1" outlineLevel="3">
-      <c r="G106" s="3" t="s">
+      <c r="I106" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J106" s="2"/>
+      <c r="K106" s="10"/>
+    </row>
+    <row r="107" spans="1:11" hidden="1" outlineLevel="3">
+      <c r="G107" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="I106" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="J106" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="K106" s="10"/>
-    </row>
-    <row r="107" spans="3:11" hidden="1" outlineLevel="3">
-      <c r="G107" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="I107" s="4" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J107" s="4" t="s">
         <v>4</v>
       </c>
       <c r="K107" s="10"/>
     </row>
-    <row r="108" spans="3:11" hidden="1" outlineLevel="3">
-      <c r="E108" s="3" t="s">
+    <row r="108" spans="1:11" hidden="1" outlineLevel="3">
+      <c r="G108" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I108" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="J108" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="K108" s="10"/>
+    </row>
+    <row r="109" spans="1:11" hidden="1" outlineLevel="3">
+      <c r="E109" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="G108" s="3"/>
-      <c r="I108" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="J108" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="K108" s="10"/>
-    </row>
-    <row r="109" spans="3:11" hidden="1" outlineLevel="3">
-      <c r="E109" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="I109" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="J109" s="2"/>
+      <c r="G109" s="3"/>
+      <c r="I109" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J109" s="4" t="s">
+        <v>8</v>
+      </c>
       <c r="K109" s="10"/>
     </row>
-    <row r="110" spans="3:11" hidden="1" outlineLevel="3">
-      <c r="F110" s="5" t="s">
+    <row r="110" spans="1:11" hidden="1" outlineLevel="3">
+      <c r="E110" s="5" t="s">
         <v>82</v>
       </c>
       <c r="I110" s="2" t="s">
@@ -4421,70 +4512,83 @@
       <c r="J110" s="2"/>
       <c r="K110" s="10"/>
     </row>
-    <row r="111" spans="3:11" hidden="1" outlineLevel="3">
-      <c r="G111" s="3" t="s">
+    <row r="111" spans="1:11" hidden="1" outlineLevel="3">
+      <c r="F111" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="I111" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J111" s="2"/>
+      <c r="K111" s="10"/>
+    </row>
+    <row r="112" spans="1:11" hidden="1" outlineLevel="3">
+      <c r="G112" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="I111" s="4" t="s">
+      <c r="I112" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="J111" s="4" t="s">
+      <c r="J112" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="K111" s="10"/>
-    </row>
-    <row r="112" spans="3:11" hidden="1" outlineLevel="3">
-      <c r="G112" s="3" t="s">
+      <c r="K112" s="10"/>
+    </row>
+    <row r="113" spans="2:12" hidden="1" outlineLevel="3">
+      <c r="G113" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="I112" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="J112" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="K112" s="10"/>
-    </row>
-    <row r="113" spans="2:12" collapsed="1">
-      <c r="B113" s="3" t="s">
-        <v>88</v>
-      </c>
       <c r="I113" s="4" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="J113" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="K113" s="10" t="s">
-        <v>279</v>
-      </c>
-      <c r="L113" s="40"/>
-    </row>
-    <row r="114" spans="2:12">
+      <c r="K113" s="10"/>
+    </row>
+    <row r="114" spans="2:12" collapsed="1">
       <c r="B114" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I114" s="4" t="s">
         <v>22</v>
       </c>
       <c r="J114" s="4" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="K114" s="10" t="s">
-        <v>166</v>
-      </c>
+        <v>279</v>
+      </c>
+      <c r="L114" s="40"/>
     </row>
     <row r="115" spans="2:12">
       <c r="B115" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="I115" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J115" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="K115" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="L115" s="17" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="116" spans="2:12">
+      <c r="B116" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="I115" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="J115" s="4" t="s">
+      <c r="I116" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J116" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="K115" s="10" t="s">
+      <c r="K116" s="10" t="s">
         <v>167</v>
       </c>
     </row>
@@ -4492,14 +4596,17 @@
   <mergeCells count="1">
     <mergeCell ref="A1:H1"/>
   </mergeCells>
-  <conditionalFormatting sqref="B69:B70">
+  <conditionalFormatting sqref="B70:B71">
     <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C70">
+  <conditionalFormatting sqref="C71">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="L48" r:id="rId1" location="_2.16.840.1.113883.2.4.3.11.60.20.77.2.3.22508_20160426110457" tooltip="Link naar dit item" display="http://decor.nictiz.nl/medicatieproces/mp-html-20170601T173502/ds-2.16.840.1.113883.2.4.3.11.60.20.77.1.3-2016-06-01T000000.html - _2.16.840.1.113883.2.4.3.11.60.20.77.2.3.22508_20160426110457"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -4507,7 +4614,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N78"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
@@ -4529,16 +4636,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="18" customHeight="1">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="54" t="s">
         <v>152</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
       <c r="I1" s="1" t="s">
         <v>132</v>
       </c>
@@ -5519,8 +5626,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K76" sqref="K76"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5535,19 +5642,20 @@
     <col min="8" max="8" width="22.28515625" customWidth="1"/>
     <col min="10" max="10" width="12.42578125" customWidth="1"/>
     <col min="11" max="11" width="54.7109375" customWidth="1"/>
+    <col min="12" max="12" width="102.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="54" t="s">
         <v>152</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
       <c r="I1" s="1" t="s">
         <v>132</v>
       </c>
@@ -5586,6 +5694,9 @@
       <c r="K3" s="46" t="s">
         <v>323</v>
       </c>
+      <c r="L3" s="55" t="s">
+        <v>376</v>
+      </c>
     </row>
     <row r="4" spans="1:12">
       <c r="B4" s="3" t="s">
@@ -5742,7 +5853,7 @@
       <c r="J15" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="K15" s="54" t="s">
+      <c r="K15" s="53" t="s">
         <v>216</v>
       </c>
     </row>
@@ -6546,7 +6657,7 @@
       <c r="J74" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="K74" s="53" t="s">
+      <c r="K74" s="52" t="s">
         <v>216</v>
       </c>
     </row>
@@ -6624,16 +6735,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="14.45" customHeight="1">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="54" t="s">
         <v>152</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
       <c r="I1" s="1" t="s">
         <v>132</v>
       </c>
@@ -7143,16 +7254,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="54" t="s">
         <v>152</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
       <c r="I1" s="1" t="s">
         <v>132</v>
       </c>

</xml_diff>